<commit_message>
Clean up, added datasheets
</commit_message>
<xml_diff>
--- a/DC-Power-Supply-BOM.xlsx
+++ b/DC-Power-Supply-BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\DC-Power-Supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B52E17A-A1C5-450B-981F-ED029BA5BDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952556C3-BC18-4453-A958-9BF22524F897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,9 +150,6 @@
     <t>https://www.adafruit.com/product/562</t>
   </si>
   <si>
-    <t>LM317T Voltage Regulator</t>
-  </si>
-  <si>
     <t>497-15588-5-ND</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>BUSS MTH 5</t>
+  </si>
+  <si>
+    <t>LD1086BV-DG Voltage Regulator</t>
   </si>
 </sst>
 </file>
@@ -629,8 +629,8 @@
   <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,10 +761,10 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
@@ -779,8 +779,8 @@
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>40</v>
+      <c r="H6" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -827,13 +827,13 @@
     </row>
     <row r="9" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -846,7 +846,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -867,15 +867,15 @@
         <v>11.99</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -915,7 +915,7 @@
         <v>9.59</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -938,10 +938,10 @@
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
@@ -957,12 +957,12 @@
         <v>0.94</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -978,7 +978,7 @@
         <v>6.82</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1092,7 +1092,7 @@
         <v>0.5</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1116,15 +1116,15 @@
         <v>0.5</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
         <v>24</v>
@@ -1140,15 +1140,15 @@
         <v>4.95</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
@@ -1164,12 +1164,12 @@
         <v>4.95</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -1696,8 +1696,10 @@
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{1B12F460-3383-4DEB-B1AC-3CBDD48300AD}"/>
     <hyperlink ref="H9" r:id="rId2" xr:uid="{B1148CFF-8D28-4431-ABDF-9833A804F09F}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{8CD51C8D-FD61-4199-A65B-C3A6E494C65B}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{4B4FB860-0F96-4E94-A62C-261650279D59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update BOM, test prints, datasheets
</commit_message>
<xml_diff>
--- a/DC-Power-Supply-BOM.xlsx
+++ b/DC-Power-Supply-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\DC-Power-Supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952556C3-BC18-4453-A958-9BF22524F897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA90B9B-A70A-4CEF-AC50-B62B8F1FE413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>Quantity</t>
   </si>
@@ -224,6 +224,24 @@
   </si>
   <si>
     <t>LD1086BV-DG Voltage Regulator</t>
+  </si>
+  <si>
+    <t>Perf Board/Screw Terminals</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07FFDCF22/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Threaded Inserts </t>
+  </si>
+  <si>
+    <t>Machine Screws</t>
+  </si>
+  <si>
+    <t>www.amazon.com/gp/product/B07HVRJW5J/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07L96KVP3/</t>
   </si>
 </sst>
 </file>
@@ -629,15 +647,15 @@
   <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="54.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.21875" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="9"/>
@@ -701,7 +719,7 @@
       </c>
       <c r="J2" s="13">
         <f>SUM(G2:G57)</f>
-        <v>79.580000000000013</v>
+        <v>95.570000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -956,7 +974,7 @@
         <f t="shared" si="0"/>
         <v>0.94</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1001,7 +1019,7 @@
         <f t="shared" si="0"/>
         <v>2.95</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1219,21 +1237,60 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9">
+        <v>15.99</v>
+      </c>
       <c r="G29" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>15.99</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
       <c r="G30" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H30" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0</v>
+      </c>
       <c r="G31" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1698,8 +1755,13 @@
     <hyperlink ref="H9" r:id="rId2" xr:uid="{B1148CFF-8D28-4431-ABDF-9833A804F09F}"/>
     <hyperlink ref="H6" r:id="rId3" xr:uid="{8CD51C8D-FD61-4199-A65B-C3A6E494C65B}"/>
     <hyperlink ref="H10" r:id="rId4" xr:uid="{4B4FB860-0F96-4E94-A62C-261650279D59}"/>
+    <hyperlink ref="H22" r:id="rId5" xr:uid="{022F960B-E847-4476-B98B-316CB071F214}"/>
+    <hyperlink ref="H17" r:id="rId6" xr:uid="{7665ADB7-C4E2-4648-BF25-C502DCB097B6}"/>
+    <hyperlink ref="H15" r:id="rId7" xr:uid="{813FF583-1931-453B-A417-DD01DA17082D}"/>
+    <hyperlink ref="H31" r:id="rId8" xr:uid="{F27E4100-42F2-4B3A-B2A1-196BC8DB4B1F}"/>
+    <hyperlink ref="H30" r:id="rId9" xr:uid="{BB643C74-132D-4334-95D0-1A8AF6901975}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed - added photos
</commit_message>
<xml_diff>
--- a/DC-Power-Supply-BOM.xlsx
+++ b/DC-Power-Supply-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\DC-Power-Supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF46B91-A4BD-4493-9CFF-B3C16D0180D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A27CBF-AAC2-4B72-A64F-BD85A338A314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,8 +656,8 @@
   <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,7 +921,7 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
@@ -941,7 +941,7 @@
         <f t="shared" si="0"/>
         <v>9.59</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="7" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1787,8 +1787,9 @@
     <hyperlink ref="H15" r:id="rId7" xr:uid="{813FF583-1931-453B-A417-DD01DA17082D}"/>
     <hyperlink ref="H31" r:id="rId8" xr:uid="{F27E4100-42F2-4B3A-B2A1-196BC8DB4B1F}"/>
     <hyperlink ref="H30" r:id="rId9" xr:uid="{BB643C74-132D-4334-95D0-1A8AF6901975}"/>
+    <hyperlink ref="H13" r:id="rId10" xr:uid="{71775749-9034-4F1B-A30C-0645F671C772}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>